<commit_message>
202501 - Hoan thanh che do thymleaf
</commit_message>
<xml_diff>
--- a/src/main/resources/static/image/IVC-Realtor-Image/Gmail-MKT-Image/Users.xlsx
+++ b/src/main/resources/static/image/IVC-Realtor-Image/Gmail-MKT-Image/Users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -27,43 +27,40 @@
     <t>gmail</t>
   </si>
   <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>nguyễn công1</t>
-  </si>
-  <si>
-    <t>trai</t>
-  </si>
-  <si>
-    <t>công1trai</t>
-  </si>
-  <si>
-    <t>nguyễncông2</t>
-  </si>
-  <si>
-    <t>gái</t>
-  </si>
-  <si>
-    <t>công2gái</t>
-  </si>
-  <si>
-    <t>nguyễncông3</t>
-  </si>
-  <si>
-    <t>già</t>
-  </si>
-  <si>
-    <t>công3già</t>
-  </si>
-  <si>
-    <t>nguyễncông4</t>
-  </si>
-  <si>
-    <t>trẻ</t>
-  </si>
-  <si>
-    <t>công4trẻ</t>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Thành Côngdncv</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>nguyenthanhcong.dn.cv@gmail.com</t>
+  </si>
+  <si>
+    <t>Thành Công120620</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>nguyenthanhcong120620@gmail.com</t>
+  </si>
+  <si>
+    <t>Thành Côngivcgroup</t>
+  </si>
+  <si>
+    <t>fm</t>
+  </si>
+  <si>
+    <t>cong.nt.ivcgroup@gmail.com</t>
+  </si>
+  <si>
+    <t>Thành Côngdev126</t>
+  </si>
+  <si>
+    <t>nguyenthanhcong.dev.126@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -80,7 +77,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -321,7 +317,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="25" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="13.0"/>
+    <col customWidth="1" min="2" max="2" width="8.71"/>
+    <col customWidth="1" min="3" max="3" width="32.14"/>
+    <col customWidth="1" min="4" max="25" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -334,7 +333,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -342,57 +341,49 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>252.0</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1">
-        <v>67876.0</v>
-      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
-        <v>345235.0</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1">
-        <v>361234.0</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1"/>

</xml_diff>